<commit_message>
Update modal analysis, netlist functions, user data
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55FC088-5439-4A79-AE2C-162E0A5389D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797F8C82-2F09-4B19-A8CB-808579FDE2D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Zbranch = R+wL+1/(wC+G)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PGi and QGi are in generator convention. PLi and QLi are in load convention.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -124,10 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B/2 (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>X (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,10 +128,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>G/2 (pu)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1-Initial step, 2-Every step</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -301,10 +289,6 @@
   </si>
   <si>
     <t>theta (rad)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customer data:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -516,15 +500,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>All self branch HAT TO be set, even with a very small value of wC or G.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>For active device (SG, VSI, etc), please use PGi and QGi. For load, please use PLi and QLi.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>There is a pi-circuit between two buses, i.e., a series RX impedance with parallel BG at two terminals.</t>
+    <t>Enable (participation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-Disable, 1-Enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The branches can be listed in arbitrary order.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User data:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B (pu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, a pi-circuit between two buses, i.e., series R+jX impedance with parallel G/2+jB/2 admittance at two terminals.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In this form, Zbranch = R+jwL+1/(G+jwC)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -626,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -642,7 +646,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -930,7 +933,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -952,7 +955,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -962,49 +965,49 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
@@ -1146,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1170,7 +1173,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
@@ -1180,7 +1183,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -1190,174 +1193,174 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
+      <c r="H16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E16" t="s">
+      <c r="I16" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="F16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
-      <c r="B21" s="12" t="s">
-        <v>107</v>
+      <c r="B21" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" t="s">
         <v>91</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E21" t="s">
+      <c r="K21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F21" t="s">
+      <c r="L21" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="G21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
-      <c r="B22" s="13" t="s">
-        <v>99</v>
+      <c r="B22" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1367,7 +1370,7 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1377,16 +1380,16 @@
     <row r="24" spans="1:12" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1396,32 +1399,32 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
@@ -1533,7 +1536,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1546,12 +1549,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -1565,7 +1568,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -1573,7 +1576,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1581,7 +1584,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1596,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1620,12 +1623,12 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -1635,53 +1638,71 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>59</v>
+      <c r="C10">
+        <v>0.01</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0.01</v>
@@ -1701,10 +1722,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0.01</v>
@@ -1727,7 +1748,7 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>0.01</v>
@@ -1742,38 +1763,38 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0.3</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F14">
+        <v>0.6</v>
       </c>
       <c r="G14">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1793,10 +1814,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1808,7 +1829,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F16">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1816,10 +1837,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1831,32 +1852,9 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F17">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="F18">
-        <v>0.05</v>
-      </c>
-      <c r="G18">
         <v>1</v>
       </c>
     </row>
@@ -1869,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1882,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -1897,55 +1895,60 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>43</v>
+      <c r="A6" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
+      <c r="A7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="5">
-        <v>0</v>
+      <c r="A8" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>66</v>
+      <c r="A9" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1957,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1970,134 +1973,145 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test SingleMachineInfiniteBus for dc
The single-grid-following-buck-infinite-bus system works!
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2453B9-14A9-4950-AFE0-9D8470CF76C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A890BE52-9671-433D-BFEB-97C9E5DAEAD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -510,19 +510,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>% 0000-1000: AC device</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>% 1000-1999: DC device</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2001: AC-DC interlink converter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>% 2000-2999: Hybrid device</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -610,6 +598,18 @@
   </si>
   <si>
     <t>The dc and hybrid devices support default data only for now.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>% 0000-0100: AC device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>% 1000-1100: DC device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>% 2000-2100: Hybrid device</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -1368,7 +1368,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -1403,17 +1403,17 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.4">
@@ -1450,17 +1450,17 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
@@ -1505,7 +1505,7 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="28" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
         <v>63</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B32" s="8" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
@@ -1568,35 +1568,35 @@
     </row>
     <row r="35" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B35" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
         <v>129</v>
       </c>
-      <c r="C35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" t="s">
-        <v>132</v>
-      </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B36" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B37" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
@@ -1606,12 +1606,12 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B40" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.4">
@@ -1641,7 +1641,7 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B46" s="8" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.4">
@@ -1656,7 +1656,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B49" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add dc and hybrid ac-dc
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DDD41A-B670-40F2-9144-0172F785E70F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AC7D03-C35D-4B1A-9C45-C67AA9CF0D24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="141">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,10 +160,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-Gauss-Seidel, 2-Newtown-Raphson</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0-No, 1-Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -201,10 +197,6 @@
   </si>
   <si>
     <t>Enable (print output)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable (plot swing)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -630,6 +622,31 @@
   </si>
   <si>
     <t>2002: vac control (grid-forming at ac side)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1-Gauss-Seidel, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2-Newton-Raphson</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Newton-Raphson power flow method can be used for pure ac grids only.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1083,17 +1100,17 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
@@ -1108,26 +1125,26 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>23</v>
@@ -1148,10 +1165,10 @@
         <v>28</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -1317,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -1361,12 +1378,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1376,168 +1393,168 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B14" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
         <v>75</v>
       </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B19" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>66</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>67</v>
       </c>
-      <c r="E20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
         <v>70</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>72</v>
       </c>
-      <c r="F25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" t="s">
-        <v>74</v>
-      </c>
       <c r="H25" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="L25" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="L25" s="9" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1546,7 +1563,7 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B27" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1555,15 +1572,15 @@
     </row>
     <row r="28" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B29" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1572,162 +1589,162 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B30" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B31" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B32" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B33" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B34" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="B35" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H35" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B36" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B37" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B38" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B40" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B41" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B42" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B43" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B44" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B45" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B46" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B47" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B48" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B49" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B50" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B51" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B52" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B53" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.4">
@@ -1859,27 +1876,27 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -1894,15 +1911,15 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
@@ -1917,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -2045,12 +2062,12 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -2070,15 +2087,15 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -2093,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -2310,7 +2327,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -2324,7 +2341,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
@@ -2332,7 +2349,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2340,7 +2357,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2355,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2368,145 +2385,144 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve the grid-following inverter class
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB6B155-EE44-448F-8173-2F5DBA81DC31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE43D0B-DE8E-4752-9A0C-04661D3A49D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -689,7 +689,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19: PR controlled</t>
+    <t>19: stationary frame modeling</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
+      <c r="B25" s="17" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify Modal analysis part
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45992AB-856B-4365-B042-5B399A62ABC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8204171-73D2-4CC4-B2A8-FC8C26014A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -609,7 +609,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -620,7 +620,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -698,19 +698,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -719,7 +719,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -727,7 +727,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -735,7 +735,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -743,14 +743,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -758,7 +758,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -766,7 +766,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -794,7 +794,7 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1104,71 +1104,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.46484375" customWidth="1"/>
-    <col min="6" max="6" width="10.9296875" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
-    <col min="10" max="10" width="11.1328125" customWidth="1"/>
-    <col min="11" max="11" width="10.1328125" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12">
       <c r="A3" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1373,70 +1373,70 @@
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.86328125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.53125" customWidth="1"/>
-    <col min="10" max="10" width="17.3984375" customWidth="1"/>
-    <col min="11" max="11" width="17.1328125" customWidth="1"/>
-    <col min="12" max="12" width="17.9296875" customWidth="1"/>
-    <col min="13" max="13" width="14.46484375" customWidth="1"/>
-    <col min="14" max="14" width="13.1328125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="B10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1444,31 +1444,31 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="B11" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="B12" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="B13" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="B14" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
@@ -1485,32 +1485,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12">
       <c r="B17" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12">
       <c r="B18" s="17" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12">
       <c r="B19" s="15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12">
       <c r="B20" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="29.25" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
@@ -1537,32 +1537,32 @@
       </c>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12">
       <c r="B22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12">
       <c r="B23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12">
       <c r="B24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:12">
       <c r="B25" s="17" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12">
       <c r="B26" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="27.4" customHeight="1">
       <c r="B27" s="10" t="s">
         <v>78</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12">
       <c r="B28" s="11" t="s">
         <v>126</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12">
       <c r="B29" s="8" t="s">
         <v>103</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:12" ht="34.5" customHeight="1">
       <c r="B30" s="7" t="s">
         <v>106</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12">
       <c r="B31" s="8" t="s">
         <v>103</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12">
       <c r="B32" s="3" t="s">
         <v>107</v>
       </c>
@@ -1640,27 +1640,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:8">
       <c r="B33" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:8">
       <c r="B34" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:8">
       <c r="B35" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:8">
       <c r="B36" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:8" ht="30">
       <c r="B37" s="12" t="s">
         <v>123</v>
       </c>
@@ -1683,72 +1683,72 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:8">
       <c r="B38" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:8">
       <c r="B39" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:8">
       <c r="B40" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:8">
       <c r="B41" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:8">
       <c r="B42" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:8">
       <c r="B43" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:8">
       <c r="B44" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:8">
       <c r="B45" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:8">
       <c r="B46" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:8">
       <c r="B47" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:8">
       <c r="B48" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10">
       <c r="B49" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10">
       <c r="B50" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" ht="30">
       <c r="B51" s="8" t="s">
         <v>127</v>
       </c>
@@ -1777,32 +1777,32 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10">
       <c r="B52" s="13" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10">
       <c r="B53" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10">
       <c r="B54" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10">
       <c r="B55" s="16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10">
       <c r="A56" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
         <v>90</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>4</v>
       </c>
@@ -1925,62 +1925,62 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2110,53 +2110,53 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2378,25 +2378,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2440,36 +2440,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>55</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2536,18 +2536,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2580,12 +2580,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>83</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
modify Modal analysis part (#10)
In this pull request, the codes in Modal Analysis are updated to fit the latest version of toolbox.

Co-authored-by: yuezhu71 <yz34218@ic.ac.uk>
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45992AB-856B-4365-B042-5B399A62ABC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8204171-73D2-4CC4-B2A8-FC8C26014A5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -609,7 +609,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -620,7 +620,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -698,19 +698,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -719,7 +719,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -727,7 +727,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -735,7 +735,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -743,14 +743,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -758,7 +758,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -766,7 +766,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -794,7 +794,7 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1104,71 +1104,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.46484375" customWidth="1"/>
-    <col min="6" max="6" width="10.9296875" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
-    <col min="10" max="10" width="11.1328125" customWidth="1"/>
-    <col min="11" max="11" width="10.1328125" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12">
       <c r="A3" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1373,70 +1373,70 @@
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.86328125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.53125" customWidth="1"/>
-    <col min="10" max="10" width="17.3984375" customWidth="1"/>
-    <col min="11" max="11" width="17.1328125" customWidth="1"/>
-    <col min="12" max="12" width="17.9296875" customWidth="1"/>
-    <col min="13" max="13" width="14.46484375" customWidth="1"/>
-    <col min="14" max="14" width="13.1328125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="B10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1444,31 +1444,31 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="B11" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="B12" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="B13" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="B14" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
@@ -1485,32 +1485,32 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12">
       <c r="B17" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12">
       <c r="B18" s="17" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12">
       <c r="B19" s="15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12">
       <c r="B20" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="29.25" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>63</v>
       </c>
@@ -1537,32 +1537,32 @@
       </c>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12">
       <c r="B22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12">
       <c r="B23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12">
       <c r="B24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:12">
       <c r="B25" s="17" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12">
       <c r="B26" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="27.4" customHeight="1">
       <c r="B27" s="10" t="s">
         <v>78</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12">
       <c r="B28" s="11" t="s">
         <v>126</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12">
       <c r="B29" s="8" t="s">
         <v>103</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:12" ht="34.5" customHeight="1">
       <c r="B30" s="7" t="s">
         <v>106</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12">
       <c r="B31" s="8" t="s">
         <v>103</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12">
       <c r="B32" s="3" t="s">
         <v>107</v>
       </c>
@@ -1640,27 +1640,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:8">
       <c r="B33" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:8">
       <c r="B34" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:8">
       <c r="B35" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:8">
       <c r="B36" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:8" ht="30">
       <c r="B37" s="12" t="s">
         <v>123</v>
       </c>
@@ -1683,72 +1683,72 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:8">
       <c r="B38" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:8">
       <c r="B39" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:8">
       <c r="B40" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:8">
       <c r="B41" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:8">
       <c r="B42" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:8">
       <c r="B43" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:8">
       <c r="B44" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:8">
       <c r="B45" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:8">
       <c r="B46" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:8">
       <c r="B47" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:8">
       <c r="B48" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10">
       <c r="B49" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10">
       <c r="B50" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" ht="30">
       <c r="B51" s="8" t="s">
         <v>127</v>
       </c>
@@ -1777,32 +1777,32 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10">
       <c r="B52" s="13" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10">
       <c r="B53" s="13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10">
       <c r="B54" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10">
       <c r="B55" s="16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10">
       <c r="A56" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
         <v>90</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1861,7 +1861,7 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>4</v>
       </c>
@@ -1925,62 +1925,62 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2110,53 +2110,53 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>3</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2378,25 +2378,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2440,36 +2440,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>55</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2536,18 +2536,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2580,12 +2580,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>83</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Update the parameter transfer of the grid-following inverter
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656B22E2-2211-45F8-A15A-6E10D4E5146B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739FEB1C-D447-40A6-91F6-2E8AF4D8561C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2440,7 +2440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Saturation and Load Impulse
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8139A1D0-8A38-4191-B6B4-F77A1D9FC906}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B254A08E-EB69-4B87-9579-264EA9302E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1369,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>